<commit_message>
Can now handle unlimited rows of campaigns
</commit_message>
<xml_diff>
--- a/TheTradeDesk API Example_5.5.15v2.xlsx
+++ b/TheTradeDesk API Example_5.5.15v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="560" windowWidth="25600" windowHeight="16060" tabRatio="868"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="868"/>
   </bookViews>
   <sheets>
     <sheet name="POST CAMPAIGN (new)" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="90">
   <si>
     <t>API REQUEST</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Function</t>
   </si>
   <si>
-    <t>New Campaign Name</t>
-  </si>
-  <si>
     <t>Create a new Adgroup</t>
   </si>
   <si>
@@ -287,6 +284,18 @@
   </si>
   <si>
     <t>https://api.thetradedesk.com/v3/doc/api/put-campaign</t>
+  </si>
+  <si>
+    <t>46k3nk3</t>
+  </si>
+  <si>
+    <t>T-Mobile</t>
+  </si>
+  <si>
+    <t>Verizon</t>
+  </si>
+  <si>
+    <t>asdffbe32</t>
   </si>
 </sst>
 </file>
@@ -380,7 +389,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="62">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -441,6 +450,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -471,7 +481,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="62">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -503,6 +513,7 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -870,7 +881,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -883,7 +894,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -902,52 +913,52 @@
         <v>3</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1">
       <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="J4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="L4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="4" customFormat="1">
       <c r="B5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>5</v>
+        <v>87</v>
       </c>
       <c r="F5" s="4">
         <v>1000</v>
@@ -959,10 +970,10 @@
         <v>42109</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L5" s="4">
         <v>1</v>
@@ -970,6 +981,30 @@
     </row>
     <row r="6" spans="1:12" s="4" customFormat="1">
       <c r="A6" s="10"/>
+      <c r="D6" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2000</v>
+      </c>
+      <c r="G6" s="4">
+        <v>50000</v>
+      </c>
+      <c r="H6" s="11">
+        <v>42124</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:12">
       <c r="B16" s="1"/>
@@ -1010,7 +1045,7 @@
   <sheetData>
     <row r="1" spans="2:9">
       <c r="C1" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="2:9">
@@ -1018,7 +1053,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:9">
@@ -1026,42 +1061,42 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:9">
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:9" s="4" customFormat="1">
       <c r="B5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="4">
         <v>1000</v>
@@ -1098,7 +1133,7 @@
   <sheetData>
     <row r="1" spans="2:14">
       <c r="C1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="2:14">
@@ -1106,7 +1141,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1119,10 +1154,10 @@
     </row>
     <row r="3" spans="2:14">
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
@@ -1135,17 +1170,17 @@
     </row>
     <row r="4" spans="2:14">
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -1185,7 +1220,7 @@
   <sheetData>
     <row r="1" spans="2:7">
       <c r="C1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="2:7">
@@ -1193,33 +1228,33 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="5" spans="2:7">
@@ -1248,7 +1283,7 @@
   <sheetData>
     <row r="1" spans="2:6">
       <c r="C1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="2:6">
@@ -1256,30 +1291,30 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1304,7 +1339,7 @@
   <sheetData>
     <row r="1" spans="2:7">
       <c r="C1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="2:7">
@@ -1312,33 +1347,33 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1373,7 +1408,7 @@
   <sheetData>
     <row r="1" spans="2:28">
       <c r="C1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="2:28">
@@ -1381,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -1395,13 +1430,13 @@
     </row>
     <row r="3" spans="2:28">
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
@@ -1410,16 +1445,16 @@
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="N3" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R3" s="16"/>
       <c r="S3" s="16"/>
@@ -1428,99 +1463,99 @@
       <c r="V3" s="16"/>
       <c r="W3" s="16"/>
       <c r="X3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y3" s="4"/>
       <c r="Z3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:28" s="2" customFormat="1">
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="I4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="L4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="N4" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="R4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="S4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="T4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="U4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="V4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="W4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="W4" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="X4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y4" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="Y4" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="Z4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AA4" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="AB4" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="2:28">
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1542,7 +1577,7 @@
         <v>1.76</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O5">
         <v>123</v>
@@ -1572,7 +1607,7 @@
         <v>0</v>
       </c>
       <c r="X5" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Y5" s="1">
         <v>1</v>
@@ -1584,12 +1619,12 @@
         <v>480</v>
       </c>
       <c r="AB5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="2:28">
       <c r="E6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -1644,7 +1679,7 @@
   <sheetData>
     <row r="1" spans="2:28">
       <c r="C1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="2:28">
@@ -1652,7 +1687,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1676,13 +1711,13 @@
     </row>
     <row r="3" spans="2:28">
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
@@ -1691,16 +1726,16 @@
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="N3" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R3" s="16"/>
       <c r="S3" s="16"/>
@@ -1709,103 +1744,103 @@
       <c r="V3" s="16"/>
       <c r="W3" s="16"/>
       <c r="X3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y3" s="4"/>
       <c r="Z3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:28">
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="I4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="L4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="N4" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="R4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="S4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="T4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="U4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="V4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="W4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="W4" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="X4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y4" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="Y4" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="Z4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AA4" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="AB4" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="2:28">
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -1818,10 +1853,10 @@
         <v>3500000</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O5">
         <v>123</v>
@@ -1830,28 +1865,28 @@
         <v>1</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X5" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Y5" s="1">
         <v>1</v>
@@ -1863,15 +1898,15 @@
         <v>480</v>
       </c>
       <c r="AB5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="2:28">
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -1884,7 +1919,7 @@
         <v>3500000</v>
       </c>
       <c r="K6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O6">
         <v>345</v>

</xml_diff>